<commit_message>
Revised lab 2 rubric for 2023
</commit_message>
<xml_diff>
--- a/Labs/Lab02-Identity/Lab2IRubric-Identity+Admin.xlsx
+++ b/Labs/Lab02-Identity/Lab2IRubric-Identity+Admin.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS296N-CourseMaterials\Labs\Lab02-Identity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CE8CC3-08A6-4BEA-935E-FFE3076B0B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA85F55-3CBE-494F-B67E-6E181CD9CB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30936" yWindow="5760" windowWidth="9420" windowHeight="10632" xr2:uid="{30F55907-EC47-624F-8636-FE6181D07E02}"/>
+    <workbookView xWindow="30612" yWindow="4080" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{30F55907-EC47-624F-8636-FE6181D07E02}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="2" r:id="rId1"/>
     <sheet name="Grading" sheetId="1" r:id="rId2"/>
+    <sheet name="2023" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
   <si>
     <t>Part 1: Textbook Tutorial</t>
   </si>
@@ -463,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A5EE8C-E354-4001-86CD-B2CD9C47B920}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -781,4 +782,155 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{213C63AE-B6B2-4F88-9CFD-7FBB04B4737E}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <f>SUM(D6:D14)</f>
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <f>SUM(E6:E14)</f>
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>